<commit_message>
changed: Room Type dropmenu options to Face-to-Face or Virtual added: Face-to-Face room text input field
</commit_message>
<xml_diff>
--- a/static/files/BSBA-FM.xlsx
+++ b/static/files/BSBA-FM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FC9017-E5A1-48BA-9C8B-A3A0F17C0A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268756F2-C943-43C5-B4C0-175A6ACF2B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C503681A-46D2-4566-9B28-A025B06E37F5}"/>
   </bookViews>
@@ -716,7 +716,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>